<commit_message>
correction mineure, logo Idefix, commande PCBWAY
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4057E698-44ED-457B-B3A2-5730B55E5FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6D762F-50F8-4853-B58E-23C3334048BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14505" yWindow="-11190" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,7 +847,7 @@
       <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G8" t="s">
@@ -977,7 +977,7 @@
       <c r="E14" t="s">
         <v>32</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G14" t="s">
@@ -1037,7 +1037,7 @@
       <c r="E17" t="s">
         <v>74</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>73</v>
       </c>
       <c r="G17" t="s">
@@ -1057,7 +1057,7 @@
       <c r="E18" t="s">
         <v>77</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>75</v>
       </c>
       <c r="G18" t="s">
@@ -1096,7 +1096,7 @@
       <c r="E21" t="s">
         <v>52</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G21" t="s">
@@ -1116,7 +1116,7 @@
       <c r="E22" t="s">
         <v>53</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G22" t="s">
@@ -1156,7 +1156,7 @@
       <c r="E24" t="s">
         <v>55</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="1" t="s">
         <v>62</v>
       </c>
       <c r="G24" t="s">
@@ -1176,7 +1176,7 @@
       <c r="E25" t="s">
         <v>63</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
         <v>67</v>
       </c>
       <c r="G25" t="s">
@@ -1201,7 +1201,7 @@
       <c r="E28" t="s">
         <v>48</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G28" t="s">
@@ -1221,7 +1221,7 @@
       <c r="E29" t="s">
         <v>82</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="1" t="s">
         <v>83</v>
       </c>
       <c r="G29" t="s">
@@ -1241,7 +1241,7 @@
       <c r="E30" t="s">
         <v>80</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="1" t="s">
         <v>81</v>
       </c>
       <c r="G30" t="s">
@@ -1261,7 +1261,7 @@
       <c r="E31" t="s">
         <v>49</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="1" t="s">
         <v>68</v>
       </c>
       <c r="G31" t="s">
@@ -1281,7 +1281,7 @@
       <c r="E32" t="s">
         <v>64</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G32" t="s">
@@ -1348,10 +1348,23 @@
     <hyperlink ref="F16" r:id="rId13" xr:uid="{FB456B5E-3B77-48F7-96D1-A4E2824E9669}"/>
     <hyperlink ref="F11" r:id="rId14" xr:uid="{3B779E7A-B4D3-41A2-96C9-36BC70E5DBEB}"/>
     <hyperlink ref="F12" r:id="rId15" xr:uid="{267E1B24-1826-4BB8-B053-1E23DB68BF16}"/>
+    <hyperlink ref="F30" r:id="rId16" display="https://www.digikey.ca/en/products/detail/vishay-dale/TNPW120650R0BEEN/21556504?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbRBgDYAWakAXXwAcAXKEAZSYCcBLAOwHMQAX3xgYATgjQQSSGix5CJEAA4AzAHYADCrqMWkdlz6CRZHQFZ4MlBhz4ikUha0ACAPIALALaY9IZlYAVV5uJndkAFlsVEwAV05sYTM4JxBEzG5MJgJOOiEgA" xr:uid="{F006EB47-D20F-4E25-9596-6B2AE41ECE68}"/>
+    <hyperlink ref="F31" r:id="rId17" xr:uid="{D4495E92-BDF5-4F85-BB76-8E08A9DFE21D}"/>
+    <hyperlink ref="F25" r:id="rId18" xr:uid="{7A6EED5B-0954-44B7-A686-D388C97754E9}"/>
+    <hyperlink ref="F14" r:id="rId19" xr:uid="{77E982EC-2DB1-4194-834D-F07E7AFC9D75}"/>
+    <hyperlink ref="F32" r:id="rId20" xr:uid="{6A8021B4-4683-4C97-AACC-E362A6018541}"/>
+    <hyperlink ref="F29" r:id="rId21" xr:uid="{4B508F79-D10E-4544-B85D-639942DBC4CD}"/>
+    <hyperlink ref="F24" r:id="rId22" xr:uid="{893D169E-BF09-4717-82F2-1F0FF18FAE01}"/>
+    <hyperlink ref="F17" r:id="rId23" xr:uid="{16E5567E-1CE1-4E52-93C1-BAD704DA304A}"/>
+    <hyperlink ref="F21" r:id="rId24" xr:uid="{0592BB3D-4A2E-41D0-8CAF-75E0233A25B7}"/>
+    <hyperlink ref="F22" r:id="rId25" xr:uid="{A014B6CE-C130-4355-971F-52B31029ADE1}"/>
+    <hyperlink ref="F8" r:id="rId26" xr:uid="{3C30F9B2-23CB-46BB-883B-2E08CB62467E}"/>
+    <hyperlink ref="F18" r:id="rId27" xr:uid="{5CD34EDE-06B3-40A2-8474-5F9F0AB887F9}"/>
+    <hyperlink ref="F28" r:id="rId28" xr:uid="{01DCB403-83E6-4B82-A01E-06D51283A375}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId29"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changement BOM et choix nouvelles pièces 1206
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6D762F-50F8-4853-B58E-23C3334048BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0692DE61-3A42-4EA8-B98D-80AADE50B728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14505" yWindow="-11190" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10770" yWindow="-11190" windowWidth="10875" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
   <si>
     <t>MLX90393</t>
   </si>
@@ -213,9 +213,6 @@
     <t>cond 4,7u</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/cal-chip-electronics-inc/GMC10X7R475K10NT/24343641</t>
-  </si>
-  <si>
     <t>cond 10u</t>
   </si>
   <si>
@@ -234,21 +231,9 @@
     <t>1206(3216)</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/venkel/AGC0603X7R250-105KXP/20484944</t>
-  </si>
-  <si>
     <t>0603(1608)</t>
   </si>
   <si>
-    <t>0402(1005)</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/venkel/AGC0402X7R500-104KNP/21783535</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/venkel/AGC0402X7R500-103KNP/20484952</t>
-  </si>
-  <si>
     <t>cond 16p</t>
   </si>
   <si>
@@ -258,15 +243,6 @@
     <t>https://www.digikey.ca/en/products/detail/koa-speer-electronics-inc/RN73H2BTTD1450F100/10092754</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/yageo/RC0402JR-0710KL/726418</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/kyocera-avx/04025U160FAT2A/3079962</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/panasonic-electronic-components/ERA-2AEB152X/1706009</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/c-k/D102J12S215PQA/768267</t>
   </si>
   <si>
@@ -309,7 +285,28 @@
     <t>res 10</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/panasonic-electronic-components/ERJ-2RKF10R0X/192072</t>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/RMCF1206FT10R0/1759594</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC1206FR-0710KL/728483</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/vishay-dale/CRCW12061K50FKEAC/7928606</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/samsung-electro-mechanics/CL31B475KOHNNNE/3888840</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/samsung-electro-mechanics/CL31B105KBHNNNE/3886726</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/kemet/C1206C104K5RACTU/411248</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/CC1206KRX7R9BB103/302908</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/kemet/CBR06C160F5GAC/3473742</t>
   </si>
 </sst>
 </file>
@@ -656,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -902,7 +899,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -914,7 +911,7 @@
         <v>46</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G11" t="s">
         <v>20</v>
@@ -922,7 +919,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -934,7 +931,7 @@
         <v>47</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G12" t="s">
         <v>20</v>
@@ -954,7 +951,7 @@
         <v>28</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G13" t="s">
         <v>20</v>
@@ -1026,7 +1023,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1035,10 +1032,10 @@
         <v>0.12</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G17" t="s">
         <v>20</v>
@@ -1046,7 +1043,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1055,10 +1052,10 @@
         <v>0.13</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G18" t="s">
         <v>20</v>
@@ -1080,10 +1077,13 @@
         <v>50</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="G20" t="s">
         <v>20</v>
+      </c>
+      <c r="H20" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1094,16 +1094,16 @@
         <v>9.3060000000000004E-2</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" t="s">
         <v>56</v>
-      </c>
-      <c r="G21" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1114,16 +1114,16 @@
         <v>1.806E-2</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="G22" t="s">
         <v>20</v>
       </c>
       <c r="H22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1134,16 +1134,16 @@
         <v>8.0499999999999999E-3</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="G23" t="s">
         <v>20</v>
       </c>
       <c r="H23" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -1154,16 +1154,16 @@
         <v>1.8600000000000001E-3</v>
       </c>
       <c r="E24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="G24" t="s">
         <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1174,16 +1174,16 @@
         <v>0.33</v>
       </c>
       <c r="E25" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="G25" t="s">
         <v>20</v>
       </c>
       <c r="H25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1202,13 +1202,13 @@
         <v>48</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G28" t="s">
         <v>20</v>
       </c>
       <c r="H28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1219,16 +1219,16 @@
         <v>0.1</v>
       </c>
       <c r="E29" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G29" t="s">
         <v>20</v>
       </c>
       <c r="H29" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -1239,16 +1239,16 @@
         <v>0.91</v>
       </c>
       <c r="E30" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G30" t="s">
         <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -1262,13 +1262,13 @@
         <v>49</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="G31" t="s">
         <v>20</v>
       </c>
       <c r="H31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1279,16 +1279,16 @@
         <v>0.39</v>
       </c>
       <c r="E32" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G32" t="s">
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.3">
@@ -1342,25 +1342,25 @@
     <hyperlink ref="F9" r:id="rId7" xr:uid="{A217C864-8D85-4E7F-8E31-A6D000832483}"/>
     <hyperlink ref="F10" r:id="rId8" display="https://www.digikey.ca/en/products/detail/liteon/LTST-C190EKT/269229?utm_adgroup=Optoelectronics&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_FR_Product&amp;utm_term=&amp;productid=&amp;utm_content=Optoelectronics&amp;utm_id=go_cmp-207527465_adg-17734287065_ad-665615850161_dsa-61690520595_dev-c_ext-_prd-_sig-CjwKCAiAxKy5BhBbEiwAYiW--7P0yyd_ZjAU4lRQGIm2_UdkWn-BHCLxW32d-3Vqq0zK5Tz_EW2nKxoCz5UQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAxKy5BhBbEiwAYiW--7P0yyd_ZjAU4lRQGIm2_UdkWn-BHCLxW32d-3Vqq0zK5Tz_EW2nKxoCz5UQAvD_BwE" xr:uid="{52AEB8C1-3281-4CF0-B9F2-15F673CB6E65}"/>
     <hyperlink ref="F20" r:id="rId9" xr:uid="{4840CE78-288C-43B8-8AAE-EBD5F3CCF74D}"/>
-    <hyperlink ref="F23" r:id="rId10" xr:uid="{D384BA1F-9224-4509-8533-B710B5F9084C}"/>
-    <hyperlink ref="F15" r:id="rId11" xr:uid="{365D7651-3F25-46BE-BEB6-8284AFBEBA76}"/>
-    <hyperlink ref="F13" r:id="rId12" xr:uid="{367CB230-24EA-4773-BA42-8053506BFC2F}"/>
-    <hyperlink ref="F16" r:id="rId13" xr:uid="{FB456B5E-3B77-48F7-96D1-A4E2824E9669}"/>
-    <hyperlink ref="F11" r:id="rId14" xr:uid="{3B779E7A-B4D3-41A2-96C9-36BC70E5DBEB}"/>
-    <hyperlink ref="F12" r:id="rId15" xr:uid="{267E1B24-1826-4BB8-B053-1E23DB68BF16}"/>
-    <hyperlink ref="F30" r:id="rId16" display="https://www.digikey.ca/en/products/detail/vishay-dale/TNPW120650R0BEEN/21556504?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbRBgDYAWakAXXwAcAXKEAZSYCcBLAOwHMQAX3xgYATgjQQSSGix5CJEAA4AzAHYADCrqMWkdlz6CRZHQFZ4MlBhz4ikUha0ACAPIALALaY9IZlYAVV5uJndkAFlsVEwAV05sYTM4JxBEzG5MJgJOOiEgA" xr:uid="{F006EB47-D20F-4E25-9596-6B2AE41ECE68}"/>
-    <hyperlink ref="F31" r:id="rId17" xr:uid="{D4495E92-BDF5-4F85-BB76-8E08A9DFE21D}"/>
-    <hyperlink ref="F25" r:id="rId18" xr:uid="{7A6EED5B-0954-44B7-A686-D388C97754E9}"/>
-    <hyperlink ref="F14" r:id="rId19" xr:uid="{77E982EC-2DB1-4194-834D-F07E7AFC9D75}"/>
-    <hyperlink ref="F32" r:id="rId20" xr:uid="{6A8021B4-4683-4C97-AACC-E362A6018541}"/>
-    <hyperlink ref="F29" r:id="rId21" xr:uid="{4B508F79-D10E-4544-B85D-639942DBC4CD}"/>
-    <hyperlink ref="F24" r:id="rId22" xr:uid="{893D169E-BF09-4717-82F2-1F0FF18FAE01}"/>
-    <hyperlink ref="F17" r:id="rId23" xr:uid="{16E5567E-1CE1-4E52-93C1-BAD704DA304A}"/>
-    <hyperlink ref="F21" r:id="rId24" xr:uid="{0592BB3D-4A2E-41D0-8CAF-75E0233A25B7}"/>
-    <hyperlink ref="F22" r:id="rId25" xr:uid="{A014B6CE-C130-4355-971F-52B31029ADE1}"/>
-    <hyperlink ref="F8" r:id="rId26" xr:uid="{3C30F9B2-23CB-46BB-883B-2E08CB62467E}"/>
-    <hyperlink ref="F18" r:id="rId27" xr:uid="{5CD34EDE-06B3-40A2-8474-5F9F0AB887F9}"/>
-    <hyperlink ref="F28" r:id="rId28" xr:uid="{01DCB403-83E6-4B82-A01E-06D51283A375}"/>
+    <hyperlink ref="F15" r:id="rId10" xr:uid="{365D7651-3F25-46BE-BEB6-8284AFBEBA76}"/>
+    <hyperlink ref="F13" r:id="rId11" xr:uid="{367CB230-24EA-4773-BA42-8053506BFC2F}"/>
+    <hyperlink ref="F16" r:id="rId12" xr:uid="{FB456B5E-3B77-48F7-96D1-A4E2824E9669}"/>
+    <hyperlink ref="F11" r:id="rId13" xr:uid="{3B779E7A-B4D3-41A2-96C9-36BC70E5DBEB}"/>
+    <hyperlink ref="F12" r:id="rId14" xr:uid="{267E1B24-1826-4BB8-B053-1E23DB68BF16}"/>
+    <hyperlink ref="F30" r:id="rId15" display="https://www.digikey.ca/en/products/detail/vishay-dale/TNPW120650R0BEEN/21556504?s=N4IgjCBcoExaBjKAzAhgGwM4FMA0IB7KAbRBgDYAWakAXXwAcAXKEAZSYCcBLAOwHMQAX3xgYATgjQQSSGix5CJEAA4AzAHYADCrqMWkdlz6CRZHQFZ4MlBhz4ikUha0ACAPIALALaY9IZlYAVV5uJndkAFlsVEwAV05sYTM4JxBEzG5MJgJOOiEgA" xr:uid="{F006EB47-D20F-4E25-9596-6B2AE41ECE68}"/>
+    <hyperlink ref="F31" r:id="rId16" xr:uid="{D4495E92-BDF5-4F85-BB76-8E08A9DFE21D}"/>
+    <hyperlink ref="F14" r:id="rId17" xr:uid="{77E982EC-2DB1-4194-834D-F07E7AFC9D75}"/>
+    <hyperlink ref="F32" r:id="rId18" xr:uid="{6A8021B4-4683-4C97-AACC-E362A6018541}"/>
+    <hyperlink ref="F29" r:id="rId19" xr:uid="{4B508F79-D10E-4544-B85D-639942DBC4CD}"/>
+    <hyperlink ref="F17" r:id="rId20" xr:uid="{16E5567E-1CE1-4E52-93C1-BAD704DA304A}"/>
+    <hyperlink ref="F21" r:id="rId21" xr:uid="{0592BB3D-4A2E-41D0-8CAF-75E0233A25B7}"/>
+    <hyperlink ref="F8" r:id="rId22" xr:uid="{3C30F9B2-23CB-46BB-883B-2E08CB62467E}"/>
+    <hyperlink ref="F18" r:id="rId23" xr:uid="{5CD34EDE-06B3-40A2-8474-5F9F0AB887F9}"/>
+    <hyperlink ref="F28" r:id="rId24" xr:uid="{01DCB403-83E6-4B82-A01E-06D51283A375}"/>
+    <hyperlink ref="F24" r:id="rId25" xr:uid="{EF2E1E0E-F631-4892-9F85-9AE8EA941CBC}"/>
+    <hyperlink ref="F22" r:id="rId26" xr:uid="{9262366C-DC20-4EFC-AF06-AECC08A00C63}"/>
+    <hyperlink ref="F23" r:id="rId27" xr:uid="{0D55CF42-A654-409E-BC50-728C6C4FB019}"/>
+    <hyperlink ref="F25" r:id="rId28" xr:uid="{A9D2C898-1287-472D-8DE8-177DF69390DC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
firmware oscillateur interne :(
</commit_message>
<xml_diff>
--- a/ReceiverRF/commande.xlsx
+++ b/ReceiverRF/commande.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Desktop\GAUL\Ordinateur-de-bord\ReceiverRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0692DE61-3A42-4EA8-B98D-80AADE50B728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34F077D-8324-4879-AF56-4D2AF15BA51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10770" yWindow="-11190" windowWidth="10875" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>